<commit_message>
Improvements to side-data, assorted edits in project build
</commit_message>
<xml_diff>
--- a/tabular/curated/hhv-ncbi-curated-side-data.xlsx
+++ b/tabular/curated/hhv-ncbi-curated-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/general/HHV6-GLUE/tabular/curated/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562CA338-0ED1-404B-9E2D-483EC8F612AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6D9A7C-A86D-1743-BB81-CA68A430025C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9240" yWindow="2480" windowWidth="28040" windowHeight="17440" xr2:uid="{152BD880-3909-2046-B14F-08FB1215E865}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2109" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2105" uniqueCount="488">
   <si>
     <t>sequenceID</t>
   </si>
@@ -1479,6 +1479,24 @@
   </si>
   <si>
     <t>A4</t>
+  </si>
+  <si>
+    <t>Chr3q</t>
+  </si>
+  <si>
+    <t>Ch1q</t>
+  </si>
+  <si>
+    <t>NK1</t>
+  </si>
+  <si>
+    <t>NK2</t>
+  </si>
+  <si>
+    <t>Chr15q</t>
+  </si>
+  <si>
+    <t>NK3</t>
   </si>
 </sst>
 </file>
@@ -1873,8 +1891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21D611B1-781A-E041-9B61-F125F05C4348}">
   <dimension ref="A1:J218"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E90" sqref="E21:E90"/>
+    <sheetView tabSelected="1" topLeftCell="B175" workbookViewId="0">
+      <selection activeCell="I186" sqref="A1:J218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6820,14 +6838,14 @@
       <c r="B155" s="6" t="s">
         <v>468</v>
       </c>
-      <c r="C155" s="6" t="s">
-        <v>4</v>
+      <c r="C155" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="D155" s="6" t="s">
-        <v>4</v>
+        <v>486</v>
       </c>
       <c r="E155" s="6" t="s">
-        <v>4</v>
+        <v>487</v>
       </c>
       <c r="F155" s="6" t="s">
         <v>4</v>
@@ -8171,7 +8189,7 @@
         <v>4</v>
       </c>
       <c r="E197" s="6" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="F197" s="6" t="s">
         <v>4</v>
@@ -8356,14 +8374,14 @@
       <c r="B203" s="6" t="s">
         <v>468</v>
       </c>
-      <c r="C203" s="6" t="s">
-        <v>4</v>
+      <c r="C203" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="D203" s="6" t="s">
-        <v>4</v>
+        <v>482</v>
       </c>
       <c r="E203" s="6" t="s">
-        <v>4</v>
+        <v>484</v>
       </c>
       <c r="F203" s="6" t="s">
         <v>4</v>
@@ -8420,14 +8438,14 @@
       <c r="B205" s="6" t="s">
         <v>468</v>
       </c>
-      <c r="C205" s="6" t="s">
-        <v>4</v>
+      <c r="C205" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="D205" s="6" t="s">
-        <v>4</v>
+        <v>483</v>
       </c>
       <c r="E205" s="6" t="s">
-        <v>4</v>
+        <v>485</v>
       </c>
       <c r="F205" s="6" t="s">
         <v>4</v>
@@ -8452,14 +8470,14 @@
       <c r="B206" s="6" t="s">
         <v>468</v>
       </c>
-      <c r="C206" s="6" t="s">
-        <v>4</v>
+      <c r="C206" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="D206" s="6" t="s">
-        <v>4</v>
+        <v>483</v>
       </c>
       <c r="E206" s="6" t="s">
-        <v>4</v>
+        <v>485</v>
       </c>
       <c r="F206" s="6" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Updated curated data 22q insert
</commit_message>
<xml_diff>
--- a/tabular/curated/hhv-ncbi-curated-side-data.xlsx
+++ b/tabular/curated/hhv-ncbi-curated-side-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anna/Projects/virus/HHV6-GLUE/tabular/curated/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/general/HHV6-GLUE/tabular/curated/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD81415-DF2A-C044-8869-0E4DB5A62B82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62EE53FF-CE6A-6246-81D8-5552774E96B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="16420" xr2:uid="{152BD880-3909-2046-B14F-08FB1215E865}"/>
+    <workbookView xWindow="15620" yWindow="2480" windowWidth="28040" windowHeight="16420" xr2:uid="{152BD880-3909-2046-B14F-08FB1215E865}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2097" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2096" uniqueCount="488">
   <si>
     <t>sequenceID</t>
   </si>
@@ -1494,6 +1494,9 @@
   </si>
   <si>
     <t>lab_construct</t>
+  </si>
+  <si>
+    <t>Chr22q</t>
   </si>
 </sst>
 </file>
@@ -1888,8 +1891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21D611B1-781A-E041-9B61-F125F05C4348}">
   <dimension ref="A1:J218"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="A1:J218"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7155,11 +7158,11 @@
       <c r="B165" s="6" t="s">
         <v>465</v>
       </c>
-      <c r="C165" s="6" t="s">
-        <v>3</v>
+      <c r="C165" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="D165" s="6" t="s">
-        <v>3</v>
+        <v>487</v>
       </c>
       <c r="E165" s="6" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Added SNP recording logic
</commit_message>
<xml_diff>
--- a/tabular/curated/hhv-ncbi-curated-side-data.xlsx
+++ b/tabular/curated/hhv-ncbi-curated-side-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/general/HHV6-GLUE/tabular/curated/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNAds/HHV6-GLUE/tabular/curated/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62EE53FF-CE6A-6246-81D8-5552774E96B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD646304-02C7-D240-9E04-583622DDADC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15620" yWindow="2480" windowWidth="28040" windowHeight="16420" xr2:uid="{152BD880-3909-2046-B14F-08FB1215E865}"/>
+    <workbookView xWindow="3480" yWindow="8080" windowWidth="27880" windowHeight="17540" xr2:uid="{152BD880-3909-2046-B14F-08FB1215E865}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1891,8 +1891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21D611B1-781A-E041-9B61-F125F05C4348}">
   <dimension ref="A1:J218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="A1:J218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>